<commit_message>
added new testcases and changed to before Method for each testcase
</commit_message>
<xml_diff>
--- a/src/main/java/com/mitthsb/qa/testdata/data.xlsx
+++ b/src/main/java/com/mitthsb/qa/testdata/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pperla\eclipse-workspace\MittHSBTest\src\main\java\com\mitthsb\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C68BE49-1B26-4390-9872-F7E4AD0B94AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4759E9-D533-4DC3-8BA7-015D3802DF62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>asd00asd!</t>
   </si>
@@ -40,24 +40,6 @@
   </si>
   <si>
     <t>Admin</t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Role</t>
-  </si>
-  <si>
-    <t>192101031686</t>
-  </si>
-  <si>
-    <t>198806011642</t>
-  </si>
-  <si>
-    <t>198109231665</t>
   </si>
 </sst>
 </file>
@@ -96,7 +78,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,32 +359,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
+      <c r="A1" s="2">
+        <v>192101031686</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
+      <c r="A2" s="2">
+        <v>198806011642</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -412,35 +392,13 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
+      <c r="A3" s="2">
+        <v>198109231665</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed testcases based on role homepageTest
</commit_message>
<xml_diff>
--- a/src/main/java/com/mitthsb/qa/testdata/data.xlsx
+++ b/src/main/java/com/mitthsb/qa/testdata/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pperla\eclipse-workspace\MittHSBTest\src\main\java\com\mitthsb\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4759E9-D533-4DC3-8BA7-015D3802DF62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3C9275-9A51-4864-8C10-04CFEA05199A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Roles" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="63">
   <si>
     <t>asd00asd!</t>
   </si>
@@ -40,6 +41,186 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t>TestCase Description</t>
+  </si>
+  <si>
+    <t>TestCaseMethodName</t>
+  </si>
+  <si>
+    <t>Fv hög</t>
+  </si>
+  <si>
+    <t>Fv admin</t>
+  </si>
+  <si>
+    <t>Handl. Låg*</t>
+  </si>
+  <si>
+    <t>Handl. Hög*</t>
+  </si>
+  <si>
+    <t>Check the title is valid or not</t>
+  </si>
+  <si>
+    <t>homePageTitleTest</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSB logo is displayed </t>
+  </si>
+  <si>
+    <t>hsbLogoTest</t>
+  </si>
+  <si>
+    <t>check whether 'Nytt Fran HSB' link is displayed and clickable.</t>
+  </si>
+  <si>
+    <t>nyttLinkTest</t>
+  </si>
+  <si>
+    <t>check whether 'Mina Sidor' link is displayed and clickable.</t>
+  </si>
+  <si>
+    <t>minaSidorlinkTest</t>
+  </si>
+  <si>
+    <t>check whether 'MittUppdrage' link is displayed and clickable.</t>
+  </si>
+  <si>
+    <t>mittUpdragLinkTest</t>
+  </si>
+  <si>
+    <t>check if region/brf is displayed or not</t>
+  </si>
+  <si>
+    <t>brfDisplayTest</t>
+  </si>
+  <si>
+    <t>Check 'Ekonomi link/tab' is displayed and cickable on the page</t>
+  </si>
+  <si>
+    <t>ekonomiTabTest</t>
+  </si>
+  <si>
+    <t>Check 'Administration' is displayed and cickable on the page</t>
+  </si>
+  <si>
+    <t>adminTabTest</t>
+  </si>
+  <si>
+    <t>Check Fastigheten link/tab is displayed and cickable on the page</t>
+  </si>
+  <si>
+    <t>fastighetenTabTest</t>
+  </si>
+  <si>
+    <t>Check Dokument link/tab is displayed and cickable on the page</t>
+  </si>
+  <si>
+    <t>dokumentTabTest</t>
+  </si>
+  <si>
+    <t>Check Fakturor display</t>
+  </si>
+  <si>
+    <t>fakturorDisplayTest</t>
+  </si>
+  <si>
+    <t>Check Regigera Genvägar link and shortcuts are created /deleted</t>
+  </si>
+  <si>
+    <t>genvagarLinkTest</t>
+  </si>
+  <si>
+    <t>Check shortcuts are redirecting to proper page</t>
+  </si>
+  <si>
+    <t>EkonomiGenvagarLinkTest</t>
+  </si>
+  <si>
+    <t>Check 'gå till kalender' link is redirecting to proper page</t>
+  </si>
+  <si>
+    <t>goTillKalenderLinkTest</t>
+  </si>
+  <si>
+    <t>Check Ekonomisk oversikt graph is displayed</t>
+  </si>
+  <si>
+    <t>ekonomiOversiktGraphTest</t>
+  </si>
+  <si>
+    <t>Check if 'se alla nyherter'link is redirecting to proper page</t>
+  </si>
+  <si>
+    <t>seAllaNyheterLinkTest</t>
+  </si>
+  <si>
+    <t>click any news article to check</t>
+  </si>
+  <si>
+    <t>nyheterArticleTest</t>
+  </si>
+  <si>
+    <t>check 'stall in senaste handelser is displayed and clickable</t>
+  </si>
+  <si>
+    <t>check the Display of 'senaste 7 handelser</t>
+  </si>
+  <si>
+    <t>senatste7HandelserFrameTest</t>
+  </si>
+  <si>
+    <t>check the Display of 'senate aldre handelser</t>
+  </si>
+  <si>
+    <t>senatsteAldreHandelserFrameTest</t>
+  </si>
+  <si>
+    <t>kommande handlelser (create event in calender and check whether it gets displayed in start page</t>
+  </si>
+  <si>
+    <t>displayKalenderEventHomePageTest</t>
+  </si>
+  <si>
+    <t>stall i din  lista' link is clickable and opening a modal container popup</t>
+  </si>
+  <si>
+    <t>stallIDinListaFunctionTest</t>
+  </si>
+  <si>
+    <t>Information icon on 'LikvidaMedel Graph' is displaying valid text</t>
+  </si>
+  <si>
+    <t>informationIconLikvidaMedelGraphTest</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>maklare</t>
+  </si>
+  <si>
+    <t>brfHavare</t>
+  </si>
+  <si>
+    <t>brfHavareAdmin</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>check whether news frame is loaded</t>
+  </si>
+  <si>
+    <t>priorityNewsFrameTest</t>
+  </si>
+  <si>
+    <t>stallIDinListaLinkDisplayTest</t>
   </si>
 </sst>
 </file>
@@ -55,18 +236,62 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -75,10 +300,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -405,4 +643,898 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E473D613-A138-4DD8-8D76-3852EFF9EEC5}">
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="80.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed testcases as per the role
</commit_message>
<xml_diff>
--- a/src/main/java/com/mitthsb/qa/testdata/data.xlsx
+++ b/src/main/java/com/mitthsb/qa/testdata/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pperla\eclipse-workspace\MittHSBTest\src\main\java\com\mitthsb\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3C9275-9A51-4864-8C10-04CFEA05199A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016ED7D0-CBEF-4166-A98D-CFAD4E867D7E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="105">
   <si>
     <t>asd00asd!</t>
   </si>
@@ -221,6 +221,132 @@
   </si>
   <si>
     <t>stallIDinListaLinkDisplayTest</t>
+  </si>
+  <si>
+    <t>ekonomiPageTitleTest</t>
+  </si>
+  <si>
+    <t>Check Alla Fakturor link  is displayed and cickable on the page</t>
+  </si>
+  <si>
+    <t>validateAllaFakturorListItemTest</t>
+  </si>
+  <si>
+    <t>Check Finansiella rapporter link  is displayed and cickable on the page</t>
+  </si>
+  <si>
+    <t>validateFinansiellaRapportListItemTest</t>
+  </si>
+  <si>
+    <t>Check 'likvida medel and skulder ' graph is displayed</t>
+  </si>
+  <si>
+    <t>likvidaMedelGraphEkonomiPageTest</t>
+  </si>
+  <si>
+    <t>Check Reapport genvagar links are displayed and clickable</t>
+  </si>
+  <si>
+    <t>reportGenvagarDisplayTest</t>
+  </si>
+  <si>
+    <t>Check if 'obetalda avgifter' frame is displayed</t>
+  </si>
+  <si>
+    <t>accountsReceivablesGraphEkonomiPageTest</t>
+  </si>
+  <si>
+    <t>Check if 'disponibelt' graph is displayed</t>
+  </si>
+  <si>
+    <t>disponibelGraphEkonomiPageTest</t>
+  </si>
+  <si>
+    <t>Check if 'kassaflode' graph is displayed</t>
+  </si>
+  <si>
+    <t>cashFlowGraphEkonomiPageTest</t>
+  </si>
+  <si>
+    <t>check the functionality of 'information icon' of Graphs</t>
+  </si>
+  <si>
+    <t>InformationIconLikvidaMedelGraphTest</t>
+  </si>
+  <si>
+    <t>InformationIconRapportGenvagarFrameTest</t>
+  </si>
+  <si>
+    <t>InformationIconDisponiBeltGraphTest</t>
+  </si>
+  <si>
+    <t>InformationIconCashFlowGraphTest</t>
+  </si>
+  <si>
+    <t>Check 'CashFlow ' graph is displayed</t>
+  </si>
+  <si>
+    <t>Check 'Dispobelt ' graph is displayed</t>
+  </si>
+  <si>
+    <t>Check 'AccountsReceivables ' graph is displayed</t>
+  </si>
+  <si>
+    <t>Check Information Icon for Likvida Medel Graph is showing the right Content</t>
+  </si>
+  <si>
+    <t>Check Information Icon for Disponibelt Graph is showing the right Content</t>
+  </si>
+  <si>
+    <t>Check Information Icon for Rapport Genvagar Graph is showing the right Content</t>
+  </si>
+  <si>
+    <t>Check if one of Rapport shortcut is redirecting properly to the Iframe in Finansiella rapporter</t>
+  </si>
+  <si>
+    <t>clicksaldoRapportGenvagarTest</t>
+  </si>
+  <si>
+    <t>Check if Digital WebFaktura button in alla Fakturor list item is properly redirecting to an external page</t>
+  </si>
+  <si>
+    <t>clickDigitalWebFakturaButtonTest</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Homepage_Professional</t>
+  </si>
+  <si>
+    <t>EkonomiPage</t>
+  </si>
+  <si>
+    <t>validatesaldoRapportTest</t>
+  </si>
+  <si>
+    <t>Saldo report link is displayed or not</t>
+  </si>
+  <si>
+    <t>adminPageTitleTest</t>
+  </si>
+  <si>
+    <t>Check skapa Kalender Handelse Button functionality</t>
+  </si>
+  <si>
+    <t>skapaKalenderTest</t>
+  </si>
+  <si>
+    <t>Check Homepage whether created calender event is displayed in Homepage</t>
+  </si>
+  <si>
+    <t>check Delete Kalender functionality is working</t>
+  </si>
+  <si>
+    <t>deleteKalenderTest</t>
+  </si>
+  <si>
+    <t>AdministrationPage</t>
   </si>
 </sst>
 </file>
@@ -236,7 +362,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,12 +372,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -300,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -316,7 +436,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,19 +779,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E473D613-A138-4DD8-8D76-3852EFF9EEC5}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="84.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -693,12 +826,15 @@
       <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -728,12 +864,15 @@
       <c r="K2" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -763,12 +902,15 @@
       <c r="K3" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -798,12 +940,15 @@
       <c r="K4" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -833,12 +978,15 @@
       <c r="K5" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -868,12 +1016,15 @@
       <c r="K6" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -903,8 +1054,11 @@
       <c r="K7" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -938,8 +1092,11 @@
       <c r="K8" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
@@ -973,8 +1130,11 @@
       <c r="K9" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
@@ -1008,8 +1168,11 @@
       <c r="K10" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
@@ -1043,8 +1206,11 @@
       <c r="K11" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>30</v>
       </c>
@@ -1078,8 +1244,11 @@
       <c r="K12" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L12" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
@@ -1113,8 +1282,11 @@
       <c r="K13" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L13" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>34</v>
       </c>
@@ -1148,8 +1320,11 @@
       <c r="K14" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>36</v>
       </c>
@@ -1183,8 +1358,11 @@
       <c r="K15" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>38</v>
       </c>
@@ -1218,8 +1396,11 @@
       <c r="K16" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>40</v>
       </c>
@@ -1253,8 +1434,11 @@
       <c r="K17" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
@@ -1288,12 +1472,15 @@
       <c r="K18" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -1323,8 +1510,11 @@
       <c r="K19" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>45</v>
       </c>
@@ -1358,8 +1548,11 @@
       <c r="K20" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>47</v>
       </c>
@@ -1393,8 +1586,11 @@
       <c r="K21" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>49</v>
       </c>
@@ -1428,12 +1624,15 @@
       <c r="K22" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L22" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -1463,12 +1662,15 @@
       <c r="K23" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L23" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1498,12 +1700,15 @@
       <c r="K24" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L24" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C25" s="7" t="s">
@@ -1532,6 +1737,997 @@
       </c>
       <c r="K25" s="5" t="s">
         <v>11</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L29" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L30" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L31" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L32" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L33" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L34" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L35" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K36" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L36" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K37" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L37" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K38" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="L38" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K39" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L39" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L40" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J41" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K41" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L41" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J42" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K42" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L42" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J43" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K43" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L43" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J44" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K44" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L44" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I45" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J45" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K45" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="L45" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J46" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K46" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L46" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J47" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K47" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L47" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K48" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L48" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K49" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="L49" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L50" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Before class and added smoketest suite and regression
</commit_message>
<xml_diff>
--- a/src/main/java/com/mitthsb/qa/testdata/data.xlsx
+++ b/src/main/java/com/mitthsb/qa/testdata/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pperla\eclipse-workspace\MittHSBTest\src\main\java\com\mitthsb\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29531EE-9A8D-4349-AD93-4E5E0215F5E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C367804-6C51-4F75-A8B4-FF43D3D1105C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Roles" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Roles!$A$1:$M$73</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="159">
   <si>
     <t>asd00asd!</t>
   </si>
@@ -497,13 +500,25 @@
   </si>
   <si>
     <t>Verify whether Genvagar can be added or modified correctly</t>
+  </si>
+  <si>
+    <t>TestType</t>
+  </si>
+  <si>
+    <t>Regressoin</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>SmokeTest,Regression</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,7 +535,13 @@
     </font>
     <font>
       <sz val="9"/>
-      <color theme="5" tint="-0.249977111117893"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -596,7 +617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -634,7 +655,33 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,30 +1012,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E473D613-A138-4DD8-8D76-3852EFF9EEC5}">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="87.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="80.88671875" style="3" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" style="3" customWidth="1"/>
+    <col min="4" max="6" width="5.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="3"/>
-    <col min="12" max="12" width="17.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="3"/>
+    <col min="8" max="8" width="5.21875" style="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="30"/>
+    <col min="12" max="13" width="17.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="36" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -998,947 +1043,1022 @@
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="19" t="s">
         <v>58</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="19" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="31" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="D2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="7" t="s">
+      <c r="H2" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="31" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="D3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="7" t="s">
+      <c r="H3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="31" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="D4" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="7" t="s">
+      <c r="H4" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="31" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="D5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="7" t="s">
+      <c r="H5" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="31" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="D6" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="7" t="s">
+      <c r="H6" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="31" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="D7" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="7" t="s">
+      <c r="H7" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L7" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="31" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="6" t="s">
+      <c r="D8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="7" t="s">
+      <c r="H8" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="31" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="6" t="s">
+      <c r="D9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="7" t="s">
+      <c r="H9" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="31" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="6" t="s">
+      <c r="D10" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="7" t="s">
+      <c r="H10" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="31" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="D11" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="7" t="s">
+      <c r="H11" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="31" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="6" t="s">
+      <c r="D12" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="7" t="s">
+      <c r="H12" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="31" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="D13" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="7" t="s">
+      <c r="H13" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="31" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="6" t="s">
+      <c r="D14" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="K14" s="7" t="s">
+      <c r="H14" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="K14" s="24" t="s">
         <v>55</v>
       </c>
       <c r="L14" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="31" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="6" t="s">
+      <c r="D15" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K15" s="7" t="s">
+      <c r="H15" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="31" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="6" t="s">
+      <c r="D16" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16" s="6" t="s">
+      <c r="H16" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="20" t="s">
         <v>11</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="31" t="s">
         <v>41</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="6" t="s">
+      <c r="D17" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K17" s="7" t="s">
+      <c r="H17" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L17" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="31" t="s">
         <v>43</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="D18" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18" s="7" t="s">
+      <c r="H18" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="31" t="s">
         <v>62</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="6" t="s">
+      <c r="D19" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19" s="7" t="s">
+      <c r="H19" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="31" t="s">
         <v>46</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="6" t="s">
+      <c r="D20" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K20" s="7" t="s">
+      <c r="H20" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="31" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="6" t="s">
+      <c r="D21" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H21" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="J21" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="K21" s="10" t="s">
+      <c r="H21" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" s="25" t="s">
         <v>55</v>
       </c>
       <c r="L21" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="31" t="s">
         <v>50</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" s="6" t="s">
+      <c r="D22" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K22" s="7" t="s">
+      <c r="H22" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="31" t="s">
         <v>52</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23" s="6" t="s">
+      <c r="D23" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K23" s="7" t="s">
+      <c r="H23" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L23" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="31" t="s">
         <v>54</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" s="6" t="s">
+      <c r="D24" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K24" s="7" t="s">
+      <c r="H24" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L24" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="31" t="s">
         <v>61</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="6" t="s">
+      <c r="D25" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K25" s="7" t="s">
+      <c r="H25" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" s="24" t="s">
         <v>11</v>
       </c>
       <c r="L25" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>9</v>
       </c>
@@ -1948,35 +2068,38 @@
       <c r="C26" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="11" t="s">
+      <c r="D26" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H26" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I26" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J26" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K26" s="12" t="s">
+      <c r="H26" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26" s="26" t="s">
         <v>11</v>
       </c>
       <c r="L26" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>64</v>
       </c>
@@ -1986,35 +2109,38 @@
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="11" t="s">
+      <c r="D27" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J27" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K27" s="12" t="s">
+      <c r="H27" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="26" t="s">
         <v>11</v>
       </c>
       <c r="L27" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>66</v>
       </c>
@@ -2024,35 +2150,38 @@
       <c r="C28" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="11" t="s">
+      <c r="D28" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H28" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K28" s="12" t="s">
+      <c r="H28" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J28" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="26" t="s">
         <v>11</v>
       </c>
       <c r="L28" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>68</v>
       </c>
@@ -2062,35 +2191,38 @@
       <c r="C29" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="11" t="s">
+      <c r="D29" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K29" s="12" t="s">
+      <c r="H29" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K29" s="26" t="s">
         <v>11</v>
       </c>
       <c r="L29" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>70</v>
       </c>
@@ -2100,35 +2232,38 @@
       <c r="C30" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" s="11" t="s">
+      <c r="D30" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J30" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K30" s="12" t="s">
+      <c r="H30" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" s="26" t="s">
         <v>11</v>
       </c>
       <c r="L30" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>72</v>
       </c>
@@ -2138,35 +2273,38 @@
       <c r="C31" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="11" t="s">
+      <c r="D31" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I31" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J31" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K31" s="12" t="s">
+      <c r="H31" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" s="26" t="s">
         <v>11</v>
       </c>
       <c r="L31" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>74</v>
       </c>
@@ -2176,35 +2314,38 @@
       <c r="C32" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D32" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F32" s="11" t="s">
+      <c r="D32" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H32" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K32" s="12" t="s">
+      <c r="H32" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K32" s="26" t="s">
         <v>11</v>
       </c>
       <c r="L32" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>76</v>
       </c>
@@ -2214,35 +2355,38 @@
       <c r="C33" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F33" s="11" t="s">
+      <c r="D33" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H33" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I33" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J33" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K33" s="12" t="s">
+      <c r="H33" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K33" s="26" t="s">
         <v>11</v>
       </c>
       <c r="L33" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>82</v>
       </c>
@@ -2252,35 +2396,38 @@
       <c r="C34" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" s="11" t="s">
+      <c r="D34" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G34" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H34" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="I34" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="J34" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="K34" s="12" t="s">
+      <c r="H34" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I34" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="J34" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="K34" s="26" t="s">
         <v>55</v>
       </c>
       <c r="L34" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>83</v>
       </c>
@@ -2290,35 +2437,38 @@
       <c r="C35" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D35" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F35" s="11" t="s">
+      <c r="D35" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G35" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H35" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I35" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J35" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K35" s="12" t="s">
+      <c r="H35" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I35" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J35" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K35" s="26" t="s">
         <v>11</v>
       </c>
       <c r="L35" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M35" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>84</v>
       </c>
@@ -2328,35 +2478,38 @@
       <c r="C36" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" s="11" t="s">
+      <c r="D36" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G36" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H36" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I36" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J36" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K36" s="11" t="s">
+      <c r="H36" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K36" s="21" t="s">
         <v>11</v>
       </c>
       <c r="L36" s="11" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>85</v>
       </c>
@@ -2366,35 +2519,38 @@
       <c r="C37" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F37" s="11" t="s">
+      <c r="D37" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G37" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H37" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I37" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J37" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K37" s="12" t="s">
+      <c r="H37" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J37" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K37" s="26" t="s">
         <v>11</v>
       </c>
       <c r="L37" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>86</v>
       </c>
@@ -2404,35 +2560,38 @@
       <c r="C38" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F38" s="11" t="s">
+      <c r="D38" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G38" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H38" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I38" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J38" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K38" s="12" t="s">
+      <c r="H38" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J38" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K38" s="26" t="s">
         <v>11</v>
       </c>
       <c r="L38" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M38" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>87</v>
       </c>
@@ -2442,35 +2601,38 @@
       <c r="C39" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D39" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F39" s="11" t="s">
+      <c r="D39" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G39" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H39" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I39" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J39" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K39" s="12" t="s">
+      <c r="H39" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I39" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K39" s="26" t="s">
         <v>11</v>
       </c>
       <c r="L39" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M39" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>85</v>
       </c>
@@ -2480,35 +2642,38 @@
       <c r="C40" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F40" s="11" t="s">
+      <c r="D40" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F40" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G40" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H40" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I40" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J40" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K40" s="12" t="s">
+      <c r="H40" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J40" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K40" s="26" t="s">
         <v>11</v>
       </c>
       <c r="L40" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M40" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>88</v>
       </c>
@@ -2518,35 +2683,38 @@
       <c r="C41" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D41" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F41" s="11" t="s">
+      <c r="D41" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G41" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H41" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="I41" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="J41" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="K41" s="12" t="s">
+      <c r="H41" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I41" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="J41" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="K41" s="26" t="s">
         <v>55</v>
       </c>
       <c r="L41" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M41" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>90</v>
       </c>
@@ -2556,35 +2724,38 @@
       <c r="C42" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D42" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F42" s="11" t="s">
+      <c r="D42" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F42" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G42" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H42" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I42" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J42" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K42" s="12" t="s">
+      <c r="H42" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I42" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J42" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K42" s="26" t="s">
         <v>11</v>
       </c>
       <c r="L42" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M42" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>96</v>
       </c>
@@ -2594,35 +2765,38 @@
       <c r="C43" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D43" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F43" s="11" t="s">
+      <c r="D43" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F43" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G43" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H43" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I43" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J43" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K43" s="12" t="s">
+      <c r="H43" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I43" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J43" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K43" s="26" t="s">
         <v>11</v>
       </c>
       <c r="L43" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M43" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>145</v>
       </c>
@@ -2632,35 +2806,38 @@
       <c r="C44" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D44" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F44" s="11" t="s">
+      <c r="D44" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G44" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H44" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="I44" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="J44" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="K44" s="12" t="s">
+      <c r="H44" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I44" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="J44" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="K44" s="26" t="s">
         <v>55</v>
       </c>
       <c r="L44" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M44" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>148</v>
       </c>
@@ -2670,35 +2847,38 @@
       <c r="C45" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D45" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F45" s="11" t="s">
+      <c r="D45" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F45" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H45" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I45" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J45" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K45" s="12" t="s">
+      <c r="H45" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I45" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J45" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K45" s="26" t="s">
         <v>11</v>
       </c>
       <c r="L45" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M45" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>147</v>
       </c>
@@ -2708,35 +2888,38 @@
       <c r="C46" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F46" s="11" t="s">
+      <c r="D46" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F46" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G46" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H46" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I46" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J46" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K46" s="12" t="s">
+      <c r="H46" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J46" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K46" s="26" t="s">
         <v>11</v>
       </c>
       <c r="L46" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M46" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>9</v>
       </c>
@@ -2746,35 +2929,38 @@
       <c r="C47" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D47" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F47" s="13" t="s">
+      <c r="D47" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F47" s="22" t="s">
         <v>11</v>
       </c>
       <c r="G47" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H47" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I47" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J47" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K47" s="14" t="s">
+      <c r="H47" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I47" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J47" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K47" s="27" t="s">
         <v>11</v>
       </c>
       <c r="L47" s="14" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M47" s="14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>98</v>
       </c>
@@ -2784,35 +2970,38 @@
       <c r="C48" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D48" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F48" s="13" t="s">
+      <c r="D48" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F48" s="22" t="s">
         <v>11</v>
       </c>
       <c r="G48" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H48" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="I48" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="J48" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="K48" s="14" t="s">
+      <c r="H48" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="I48" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="J48" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="K48" s="27" t="s">
         <v>55</v>
       </c>
       <c r="L48" s="14" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M48" s="14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>100</v>
       </c>
@@ -2822,35 +3011,38 @@
       <c r="C49" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F49" s="13" t="s">
+      <c r="D49" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F49" s="22" t="s">
         <v>11</v>
       </c>
       <c r="G49" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H49" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I49" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J49" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K49" s="14" t="s">
+      <c r="H49" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I49" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J49" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K49" s="27" t="s">
         <v>11</v>
       </c>
       <c r="L49" s="14" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M49" s="14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>101</v>
       </c>
@@ -2860,35 +3052,38 @@
       <c r="C50" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D50" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F50" s="13" t="s">
+      <c r="D50" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F50" s="22" t="s">
         <v>11</v>
       </c>
       <c r="G50" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H50" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I50" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J50" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K50" s="14" t="s">
+      <c r="H50" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I50" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J50" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K50" s="27" t="s">
         <v>11</v>
       </c>
       <c r="L50" s="14" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M50" s="14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
         <v>120</v>
       </c>
@@ -2898,35 +3093,38 @@
       <c r="C51" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F51" s="15" t="s">
+      <c r="D51" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G51" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H51" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I51" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J51" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K51" s="16" t="s">
+      <c r="H51" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I51" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J51" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K51" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L51" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M51" s="16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
         <v>121</v>
       </c>
@@ -2936,35 +3134,38 @@
       <c r="C52" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D52" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F52" s="15" t="s">
+      <c r="D52" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G52" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H52" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I52" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J52" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K52" s="16" t="s">
+      <c r="H52" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I52" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J52" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K52" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L52" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M52" s="16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
         <v>122</v>
       </c>
@@ -2974,35 +3175,38 @@
       <c r="C53" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D53" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" s="15" t="s">
+      <c r="D53" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G53" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H53" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I53" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J53" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K53" s="16" t="s">
+      <c r="H53" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I53" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J53" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K53" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L53" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M53" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
         <v>133</v>
       </c>
@@ -3012,35 +3216,38 @@
       <c r="C54" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D54" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F54" s="15" t="s">
+      <c r="D54" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G54" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H54" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I54" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J54" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K54" s="16" t="s">
+      <c r="H54" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I54" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J54" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K54" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L54" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M54" s="16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
         <v>134</v>
       </c>
@@ -3050,35 +3257,38 @@
       <c r="C55" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D55" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F55" s="15" t="s">
+      <c r="D55" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F55" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G55" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H55" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I55" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J55" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K55" s="16" t="s">
+      <c r="H55" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I55" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J55" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K55" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L55" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M55" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
         <v>131</v>
       </c>
@@ -3088,35 +3298,38 @@
       <c r="C56" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D56" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F56" s="15" t="s">
+      <c r="D56" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G56" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H56" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I56" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J56" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K56" s="16" t="s">
+      <c r="H56" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I56" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J56" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K56" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L56" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M56" s="16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
         <v>132</v>
       </c>
@@ -3126,35 +3339,38 @@
       <c r="C57" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D57" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F57" s="15" t="s">
+      <c r="D57" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F57" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G57" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H57" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I57" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J57" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K57" s="16" t="s">
+      <c r="H57" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I57" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J57" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K57" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L57" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M57" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
         <v>129</v>
       </c>
@@ -3164,35 +3380,38 @@
       <c r="C58" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D58" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E58" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F58" s="15" t="s">
+      <c r="D58" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F58" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G58" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H58" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I58" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J58" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K58" s="16" t="s">
+      <c r="H58" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I58" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J58" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K58" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L58" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M58" s="16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
         <v>130</v>
       </c>
@@ -3202,35 +3421,38 @@
       <c r="C59" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D59" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F59" s="15" t="s">
+      <c r="D59" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F59" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G59" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H59" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="I59" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="J59" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="K59" s="16" t="s">
+      <c r="H59" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="I59" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="J59" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="K59" s="28" t="s">
         <v>55</v>
       </c>
       <c r="L59" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M59" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
         <v>127</v>
       </c>
@@ -3240,35 +3462,38 @@
       <c r="C60" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D60" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F60" s="15" t="s">
+      <c r="D60" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F60" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G60" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H60" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I60" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J60" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K60" s="16" t="s">
+      <c r="H60" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I60" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J60" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K60" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L60" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M60" s="16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
         <v>128</v>
       </c>
@@ -3278,35 +3503,38 @@
       <c r="C61" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D61" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F61" s="15" t="s">
+      <c r="D61" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F61" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H61" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="I61" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J61" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="K61" s="15" t="s">
+      <c r="H61" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I61" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J61" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="K61" s="23" t="s">
         <v>11</v>
       </c>
       <c r="L61" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M61" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
         <v>125</v>
       </c>
@@ -3316,35 +3544,38 @@
       <c r="C62" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D62" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F62" s="15" t="s">
+      <c r="D62" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F62" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G62" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H62" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I62" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J62" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K62" s="16" t="s">
+      <c r="H62" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I62" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J62" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K62" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L62" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M62" s="16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
         <v>126</v>
       </c>
@@ -3354,35 +3585,38 @@
       <c r="C63" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D63" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F63" s="15" t="s">
+      <c r="D63" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F63" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G63" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H63" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I63" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J63" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K63" s="16" t="s">
+      <c r="H63" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I63" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J63" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K63" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L63" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M63" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="15" t="s">
         <v>123</v>
       </c>
@@ -3392,35 +3626,38 @@
       <c r="C64" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D64" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E64" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F64" s="15" t="s">
+      <c r="D64" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F64" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G64" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H64" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I64" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J64" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K64" s="16" t="s">
+      <c r="H64" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I64" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J64" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K64" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L64" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M64" s="16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
         <v>124</v>
       </c>
@@ -3430,35 +3667,38 @@
       <c r="C65" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D65" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E65" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F65" s="15" t="s">
+      <c r="D65" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F65" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G65" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H65" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I65" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J65" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K65" s="16" t="s">
+      <c r="H65" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I65" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J65" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K65" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L65" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M65" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
         <v>138</v>
       </c>
@@ -3468,35 +3708,38 @@
       <c r="C66" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D66" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E66" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F66" s="15" t="s">
+      <c r="D66" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F66" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G66" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H66" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="I66" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="J66" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="K66" s="18" t="s">
+      <c r="H66" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="I66" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="J66" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="K66" s="29" t="s">
         <v>55</v>
       </c>
       <c r="L66" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M66" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
         <v>137</v>
       </c>
@@ -3506,35 +3749,38 @@
       <c r="C67" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D67" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E67" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F67" s="15" t="s">
+      <c r="D67" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F67" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G67" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H67" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I67" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J67" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K67" s="16" t="s">
+      <c r="H67" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I67" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J67" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K67" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L67" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M67" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
         <v>136</v>
       </c>
@@ -3544,35 +3790,38 @@
       <c r="C68" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D68" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F68" s="15" t="s">
+      <c r="D68" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F68" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G68" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H68" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I68" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J68" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K68" s="16" t="s">
+      <c r="H68" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I68" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J68" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K68" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L68" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M68" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="17" t="s">
         <v>150</v>
       </c>
@@ -3582,35 +3831,38 @@
       <c r="C69" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D69" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F69" s="15" t="s">
+      <c r="D69" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F69" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G69" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H69" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I69" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J69" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K69" s="16" t="s">
+      <c r="H69" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I69" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J69" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K69" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L69" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M69" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
         <v>139</v>
       </c>
@@ -3620,35 +3872,38 @@
       <c r="C70" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D70" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F70" s="15" t="s">
+      <c r="D70" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F70" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G70" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H70" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I70" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J70" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K70" s="16" t="s">
+      <c r="H70" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I70" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J70" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K70" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L70" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M70" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
         <v>142</v>
       </c>
@@ -3658,35 +3913,38 @@
       <c r="C71" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D71" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E71" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F71" s="15" t="s">
+      <c r="D71" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F71" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G71" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H71" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I71" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J71" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K71" s="16" t="s">
+      <c r="H71" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I71" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J71" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K71" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L71" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M71" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
         <v>153</v>
       </c>
@@ -3696,35 +3954,38 @@
       <c r="C72" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D72" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E72" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F72" s="15" t="s">
+      <c r="D72" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F72" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G72" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H72" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I72" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J72" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K72" s="16" t="s">
+      <c r="H72" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I72" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J72" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K72" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L72" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M72" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
         <v>154</v>
       </c>
@@ -3734,35 +3995,39 @@
       <c r="C73" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D73" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E73" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F73" s="15" t="s">
+      <c r="D73" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E73" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F73" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G73" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H73" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I73" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J73" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K73" s="16" t="s">
+      <c r="H73" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I73" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J73" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K73" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L73" s="16" t="s">
         <v>119</v>
       </c>
+      <c r="M73" s="16" t="s">
+        <v>156</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M73" xr:uid="{4278DAC9-AE57-4872-947D-0407EDC03C85}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>